<commit_message>
got import to work
</commit_message>
<xml_diff>
--- a/uploads/imported_data.xlsx
+++ b/uploads/imported_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosey\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliss\OneDrive\Desktop\SusanDB\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB93D9D4-D922-4508-A53B-0FB8AB9BACA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D3C852-596E-43E2-BC2A-718FEEC6C53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="8170" xr2:uid="{97DC95F2-3478-49E5-8D96-4F4A29E57BC1}"/>
+    <workbookView xWindow="11555" yWindow="980" windowWidth="8080" windowHeight="9645" xr2:uid="{97DC95F2-3478-49E5-8D96-4F4A29E57BC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,18 +36,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>fav_subject</t>
-  </si>
-  <si>
-    <t>Eating</t>
-  </si>
-  <si>
-    <t>Ava Davis</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>d06edc19</t>
+  </si>
+  <si>
+    <t>Ethnicity</t>
+  </si>
+  <si>
+    <t>GPA</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>342ab1a5</t>
+  </si>
+  <si>
+    <t>Sanchez</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>3c346d6e</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Hispanic</t>
   </si>
 </sst>
 </file>
@@ -83,8 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,28 +456,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89636726-73D9-4556-9A59-ED29324B9E09}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="3" max="3" width="8.953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>3.7</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>3.82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>3.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added preview table, but broken but running late to class!!!!!!!
</commit_message>
<xml_diff>
--- a/uploads/imported_data.xlsx
+++ b/uploads/imported_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliss\OneDrive\Desktop\SusanDB\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE971CA0-83AD-4415-B946-503E0A08B484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54B3D48-B8F8-4239-A97A-AC38A407978E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11120" yWindow="980" windowWidth="8080" windowHeight="9645" xr2:uid="{97DC95F2-3478-49E5-8D96-4F4A29E57BC1}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -532,7 +532,7 @@
         <v>7</v>
       </c>
       <c r="E4">
-        <v>3.63</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished preview table implementation
</commit_message>
<xml_diff>
--- a/uploads/imported_data.xlsx
+++ b/uploads/imported_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliss\OneDrive\Desktop\SusanDB\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54B3D48-B8F8-4239-A97A-AC38A407978E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B74E4B6-B9A5-496D-958B-C3CD404D640A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11120" yWindow="980" windowWidth="8080" windowHeight="9645" xr2:uid="{97DC95F2-3478-49E5-8D96-4F4A29E57BC1}"/>
   </bookViews>
@@ -68,22 +68,22 @@
     <t>342ab1a5</t>
   </si>
   <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>3c346d6e</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Hispanic</t>
+  </si>
+  <si>
     <t>Sanchez</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>3c346d6e</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Hispanic</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -506,33 +506,33 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3">
-        <v>3.42</v>
+        <v>3.54</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4">
-        <v>3.5</v>
+        <v>3.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug with editing data
</commit_message>
<xml_diff>
--- a/uploads/imported_data.xlsx
+++ b/uploads/imported_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliss\OneDrive\Desktop\SusanDB\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosey\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B74E4B6-B9A5-496D-958B-C3CD404D640A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48EBC0A-6DC9-4B73-952F-A18FC11C29BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11120" yWindow="980" windowWidth="8080" windowHeight="9645" xr2:uid="{97DC95F2-3478-49E5-8D96-4F4A29E57BC1}"/>
+    <workbookView xWindow="1560" yWindow="2020" windowWidth="14400" windowHeight="8180" xr2:uid="{97DC95F2-3478-49E5-8D96-4F4A29E57BC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,29 +36,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>d06edc19</t>
-  </si>
-  <si>
     <t>Ethnicity</t>
   </si>
   <si>
     <t>GPA</t>
   </si>
   <si>
-    <t>White</t>
-  </si>
-  <si>
     <t>Last_Name</t>
   </si>
   <si>
-    <t>Davis</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
@@ -68,6 +59,9 @@
     <t>342ab1a5</t>
   </si>
   <si>
+    <t>Sanchez</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
@@ -81,9 +75,6 @@
   </si>
   <si>
     <t>Hispanic</t>
-  </si>
-  <si>
-    <t>Sanchez</t>
   </si>
 </sst>
 </file>
@@ -119,9 +110,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,83 +446,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89636726-73D9-4556-9A59-ED29324B9E09}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="8.953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
+      <c r="E2">
+        <v>3.82</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
       <c r="E3">
         <v>3.54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <v>3.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>